<commit_message>
this shit is literally fucking impossible
</commit_message>
<xml_diff>
--- a/descreteMath/termpaper1/курсачтаблицаЧасть2.xlsx
+++ b/descreteMath/termpaper1/курсачтаблицаЧасть2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\ITMO-Labs\descreteMath\termpaper1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137464B7-56D4-4584-A757-9330CB25C552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161291E0-FE86-412F-9CC7-B123FBC6CEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5556" yWindow="0" windowWidth="15600" windowHeight="10812" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c1" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="X21" sqref="X21"/>
@@ -15112,7 +15112,7 @@
   <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49:S52"/>
+      <selection activeCell="N1" sqref="N1:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>